<commit_message>
Change normal Formulas unit test to check for equality of 2 cells that should be equal
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/Formulas.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/Formulas.xlsx
@@ -496,7 +496,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="G2" s="0">
-        <x:f>IF(D2=F2,"Yes", "No")</x:f>
+        <x:f>IF(C2=F2,"Yes", "No")</x:f>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:7">
@@ -519,7 +519,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="G3" s="0">
-        <x:f>IF(D3=F3,"Yes", "No")</x:f>
+        <x:f>IF(C3=F3,"Yes", "No")</x:f>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:7">
@@ -542,7 +542,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="G4" s="0">
-        <x:f>IF(D4=F4,"Yes", "No")</x:f>
+        <x:f>IF(C4=F4,"Yes", "No")</x:f>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:7">

</xml_diff>

<commit_message>
Update test cases for array formulas
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/Formulas.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/Formulas.xlsx
@@ -552,6 +552,12 @@
       <x:c r="B6" s="0">
         <x:f t="array" ref="B6:B6">A2+A3</x:f>
       </x:c>
+      <x:c r="C6" s="0">
+        <x:f t="array" ref="C6:D6">TRANSPOSE(A2:A3)</x:f>
+      </x:c>
+      <x:c r="D6" s="0">
+        <x:f t="array"/>
+      </x:c>
     </x:row>
     <x:row r="10" spans="1:7">
       <x:c r="A10" s="0" t="n">

</xml_diff>